<commit_message>
accuracy changes, inverse image order
</commit_message>
<xml_diff>
--- a/webapp/static/Portfolio.xlsx
+++ b/webapp/static/Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Goliat\webapp\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54A99F0-84B3-4BD4-8D5A-69378DCE8109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB053CD-7878-411A-A888-8BC68AB813E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC03D1C2-E99C-4F24-B81E-CC33184620FD}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -141,9 +141,6 @@
     <t>Jabones y Gel</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>203 230 , 203 169</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>837 00 , 203 560</t>
+  </si>
+  <si>
+    <t>Tork® Jabones</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -675,7 +675,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
@@ -692,13 +692,13 @@
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,13 +732,13 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,13 +752,13 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,13 +772,13 @@
         <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
@@ -832,13 +832,13 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
@@ -872,13 +872,13 @@
         <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -932,13 +932,13 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,13 +972,13 @@
         <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,10 +995,10 @@
         <v>32</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>29</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>31</v>
@@ -1055,10 +1055,10 @@
         <v>32</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,13 +1072,13 @@
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,10 +1095,10 @@
         <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>29</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>30</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>31</v>
@@ -1155,10 +1155,10 @@
         <v>32</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,13 +1172,13 @@
         <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1195,10 +1195,10 @@
         <v>32</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>29</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>31</v>
@@ -1255,10 +1255,10 @@
         <v>32</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,13 +1272,13 @@
         <v>23</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1295,10 +1295,10 @@
         <v>32</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
         <v>29</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
         <v>30</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>31</v>
@@ -1355,10 +1355,10 @@
         <v>32</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1372,13 +1372,13 @@
         <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,13 +1392,13 @@
         <v>23</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1412,13 +1412,13 @@
         <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,13 +1432,13 @@
         <v>18</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,13 +1452,13 @@
         <v>26</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1472,13 +1472,13 @@
         <v>23</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,13 +1492,13 @@
         <v>8</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,13 +1512,13 @@
         <v>18</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,13 +1532,13 @@
         <v>26</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,13 +1552,13 @@
         <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,13 +1572,13 @@
         <v>8</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,13 +1592,13 @@
         <v>18</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,13 +1612,13 @@
         <v>26</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E51" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1632,17 +1632,17 @@
         <v>18</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F51" xr:uid="{977F2531-7A5B-42F7-8141-39558429BE53}"/>
+  <autoFilter ref="A1:F52" xr:uid="{977F2531-7A5B-42F7-8141-39558429BE53}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 ESSITY INTERNAL</oddFooter>

</xml_diff>